<commit_message>
last sale no longer occurs at 4pm
</commit_message>
<xml_diff>
--- a/tests/simple_orders.xlsx
+++ b/tests/simple_orders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Insulin\Documents\Coding\Python Coding\cointracker-v2-git\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365962D1-A6BD-421A-9DED-659C15931963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3533D179-C701-49BA-A5FB-9E2986EFD710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10500" yWindow="4632" windowWidth="30192" windowHeight="16884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6384" yWindow="4500" windowWidth="30192" windowHeight="16884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -400,7 +400,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,7 +556,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>44621.666666666664</v>
+        <v>44621</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>

</xml_diff>